<commit_message>
Hoàn thiện hệ thống Check Orders v2.0
 Tính năng mới:
- Xử lý Excel tự động với 10 bước nghiệp vụ
- Tích hợp hoàn chỉnh với hệ thống check orders
- Menu quản lý thân thiện (menu.py)
- Công cụ kiểm tra hệ thống (test_system.py)
- Tùy chọn tạo file tổng hợp (mặc định tắt)

 Cải tiến:
- Xử lý Excel: ẩn dòng/cột, freeze panes, auto-fit
- Không làm mất dữ liệu gốc
- Báo cáo chi tiết quá trình xử lý
- Dễ mở rộng và tùy chỉnh

 File mới:
- process_excel.py: Xử lý Excel chuyên nghiệp
- menu.py: Menu quản lý hệ thống
- test_system.py: Kiểm tra và debug
- HUONG_DAN.md: Hướng dẫn chi tiết
- FINAL_SUMMARY.md: Tổng kết hệ thống

 Sẵn sàng production!
</commit_message>
<xml_diff>
--- a/input/template.xlsx
+++ b/input/template.xlsx
@@ -28,10 +28,10 @@
     <t>SLNMCD - Sản lượng Nước Mắm Cao Đạm 6 loại (Thùng)</t>
   </si>
   <si>
-    <t>Mắm HV (500&amp;750ML)</t>
-  </si>
-  <si>
-    <t>SL_NMHV500_750ML - Sản lượng Nước mắm Hương Việt 500ml &amp; 750ml (Thùng)</t>
+    <t>DHTC</t>
+  </si>
+  <si>
+    <t>DHTC - Đơn hàng thành công</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Cập nhật cho bản phát hành v2.2
</commit_message>
<xml_diff>
--- a/input/template.xlsx
+++ b/input/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Tên viết tắt</t>
   </si>
@@ -22,16 +22,13 @@
     <t>Tên báo cáo</t>
   </si>
   <si>
-    <t>NMCD 6 loại</t>
+    <t>UTNHQTT</t>
   </si>
   <si>
-    <t>SLNMCD - Sản lượng Nước Mắm Cao Đạm 6 loại (Thùng)</t>
+    <t>SLUTNHQ90190 - Sản lượng UTN HQ truyền thống 90g - 190g</t>
   </si>
   <si>
-    <t>DHTC</t>
-  </si>
-  <si>
-    <t>DHTC - Đơn hàng thành công</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -68,9 +65,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -384,11 +384,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="70.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="70.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -404,12 +404,12 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ghi đè: cập nhật process_excel.py, check_oder.py, template.xlsx, xóa requirements.txt
</commit_message>
<xml_diff>
--- a/input/template.xlsx
+++ b/input/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tên viết tắt</t>
   </si>
@@ -28,7 +28,10 @@
     <t>SLUTNHQ90190 - Sản lượng UTN HQ truyền thống 90g - 190g</t>
   </si>
   <si>
-    <t/>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>DHTC - Đơn hàng thành công</t>
   </si>
 </sst>
 </file>
@@ -65,12 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -384,11 +384,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="70.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="70.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -404,12 +404,12 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>